<commit_message>
Edited the task durations and the readme file
</commit_message>
<xml_diff>
--- a/tasl list.xlsx
+++ b/tasl list.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\WebstormProjects\UI-UX-Challange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B909547A-1517-4D1B-89BD-F5EF7883D2E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2063AED2-B82C-427D-963D-7C07ECE5C644}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{ADF847E1-C258-48FC-8B6F-E50355BED00F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Capturing of data System</t>
   </si>
@@ -41,23 +41,73 @@
     <t>AI integration to give predictions and patterns</t>
   </si>
   <si>
-    <t>Build IoT Devices</t>
-  </si>
-  <si>
     <t>monitor the growth process of flower farm</t>
   </si>
   <si>
     <t>give insights</t>
   </si>
   <si>
-    <t>Building the Software</t>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Improve UI/UX</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Designed a manual input UI</t>
+  </si>
+  <si>
+    <t>Total Duration</t>
+  </si>
+  <si>
+    <t>A. Building the Software</t>
+  </si>
+  <si>
+    <t>B. Build IoT Devices</t>
+  </si>
+  <si>
+    <t>C: Integrating Software and Devices</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Duration
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Days)</t>
+    </r>
+  </si>
+  <si>
+    <t>Due
+Date</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +124,27 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -99,15 +170,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -417,70 +545,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C601AF9-3119-4103-A620-C7E1332B7465}">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="57.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="D3" s="8">
+        <v>43636</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>43638</v>
+      </c>
+      <c r="E4" s="9">
+        <f ca="1">IF(((TODAY()-D3)/C4)&gt;=0,(TODAY()-D3)/C4,0)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="D5" s="8">
+        <f>D3+C5</f>
+        <v>43640</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" ref="E5:E11" ca="1" si="0">IF(((TODAY()-D4)/C5)&gt;=0,(TODAY()-D4)/C5,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" ref="D6:D11" si="1">D5+C6</f>
+        <v>43643</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="1"/>
+        <v>43647</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="C8" s="6">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="1"/>
+        <v>43654</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
         <v>3</v>
       </c>
-    </row>
+      <c r="D9" s="8">
+        <f t="shared" si="1"/>
+        <v>43657</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="1"/>
+        <v>43663</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5">
+        <f>SUM(C3:C10)</f>
+        <v>30</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="1"/>
+        <v>43693</v>
+      </c>
+      <c r="E11" s="12">
+        <f ca="1">IF(((TODAY()-D3)/C11)&gt;=0,(TODAY()-D3)/C11,0)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="E4:E11">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>75</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>